<commit_message>
add many file include GAN etc
</commit_message>
<xml_diff>
--- a/simulation/one-taxi/output/100次训练结果比较/司机收入表.xlsx
+++ b/simulation/one-taxi/output/100次训练结果比较/司机收入表.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E401DA1B-0D74-4841-83B9-ADB8D4619ED8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AC0D6F-7E19-4C4F-AA47-532ADCACA23D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="3570" windowWidth="21600" windowHeight="11370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>DQN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,12 +48,25 @@
     <t>计算</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Edge-DQN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>司机收入-运行天数</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +76,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -89,10 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2323,73 +2347,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>司机收入</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>-</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>运行天数</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
+      <c:areaChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -2397,30 +2358,27 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DQN</c:v>
+                  <c:v>Edge-DQN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2459,44 +2417,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>53328.571428571398</c:v>
+                  <c:v>533.28571428571399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53509.285714285681</c:v>
+                  <c:v>535.09285714285681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53131.428571428514</c:v>
+                  <c:v>531.31428571428512</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53170.714285714224</c:v>
+                  <c:v>531.70714285714223</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53683.142857142819</c:v>
+                  <c:v>536.83142857142821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53445.476190476162</c:v>
+                  <c:v>534.45476190476165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53621.632653061199</c:v>
+                  <c:v>536.21632653061204</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53721.785714285696</c:v>
+                  <c:v>537.21785714285693</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53900.952380952353</c:v>
+                  <c:v>539.00952380952356</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54035.428571428536</c:v>
+                  <c:v>540.35428571428531</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F8E6-4B58-8807-93CF63015A1C}"/>
@@ -2508,7 +2465,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2518,20 +2475,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2570,44 +2524,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50791.428571428551</c:v>
+                  <c:v>507.91428571428548</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51617.142857142826</c:v>
+                  <c:v>516.17142857142824</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50972.380952380918</c:v>
+                  <c:v>509.72380952380917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50746.785714285666</c:v>
+                  <c:v>507.46785714285664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50692.857142857101</c:v>
+                  <c:v>506.92857142857099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50390.952380952338</c:v>
+                  <c:v>503.90952380952336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50601.836734693847</c:v>
+                  <c:v>506.01836734693848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50395.714285714261</c:v>
+                  <c:v>503.95714285714263</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50076.349206349179</c:v>
+                  <c:v>500.76349206349181</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49962.57142857142</c:v>
+                  <c:v>499.6257142857142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F8E6-4B58-8807-93CF63015A1C}"/>
@@ -2619,7 +2572,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2629,20 +2582,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2681,44 +2631,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>49284.285714285652</c:v>
+                  <c:v>492.84285714285653</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50565.714285714217</c:v>
+                  <c:v>505.65714285714216</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50994.761904761828</c:v>
+                  <c:v>509.94761904761828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50796.78571428563</c:v>
+                  <c:v>507.9678571428563</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50955.714285714217</c:v>
+                  <c:v>509.5571428571422</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50494.999999999935</c:v>
+                  <c:v>504.94999999999936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50362.040816326473</c:v>
+                  <c:v>503.62040816326476</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50248.035714285666</c:v>
+                  <c:v>502.48035714285669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50062.063492063455</c:v>
+                  <c:v>500.62063492063453</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50203.285714285681</c:v>
+                  <c:v>502.03285714285681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F8E6-4B58-8807-93CF63015A1C}"/>
@@ -2733,10 +2682,9 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="62867071"/>
         <c:axId val="71480399"/>
-      </c:lineChart>
+      </c:areaChart>
       <c:catAx>
         <c:axId val="62867071"/>
         <c:scaling>
@@ -2744,6 +2692,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time Step</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2809,6 +2812,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Income(CNY)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2842,7 +2901,7 @@
         </c:txPr>
         <c:crossAx val="62867071"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -7118,15 +7177,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8DBDF7-BCAF-4CBB-88A3-0B6D4C5632DA}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -7137,8 +7196,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -7154,8 +7222,23 @@
         <f>AVERAGE(data!D2:D11)</f>
         <v>49284.285714285652</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <f>B2/100</f>
+        <v>533.28571428571399</v>
+      </c>
+      <c r="H2">
+        <f>C2/100</f>
+        <v>507.91428571428548</v>
+      </c>
+      <c r="I2">
+        <f>D2/100</f>
+        <v>492.84285714285653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -7171,8 +7254,23 @@
         <f>AVERAGE(data!D2:D21)</f>
         <v>50565.714285714217</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G11" si="0">B3/100</f>
+        <v>535.09285714285681</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H11" si="1">C3/100</f>
+        <v>516.17142857142824</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="2">D3/100</f>
+        <v>505.65714285714216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>30</v>
       </c>
@@ -7188,8 +7286,23 @@
         <f>AVERAGE(data!D2:D31)</f>
         <v>50994.761904761828</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>531.31428571428512</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>509.72380952380917</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>509.94761904761828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>40</v>
       </c>
@@ -7205,8 +7318,23 @@
         <f>AVERAGE(data!D2:D41)</f>
         <v>50796.78571428563</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>531.70714285714223</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>507.46785714285664</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>507.9678571428563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50</v>
       </c>
@@ -7222,8 +7350,23 @@
         <f>AVERAGE(data!D2:D51)</f>
         <v>50955.714285714217</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>536.83142857142821</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>506.92857142857099</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>509.5571428571422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
@@ -7239,8 +7382,23 @@
         <f>AVERAGE(data!D2:D61)</f>
         <v>50494.999999999935</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>534.45476190476165</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>503.90952380952336</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>504.94999999999936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>70</v>
       </c>
@@ -7256,8 +7414,23 @@
         <f>AVERAGE(data!D2:D71)</f>
         <v>50362.040816326473</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>70</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>536.21632653061204</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>506.01836734693848</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>503.62040816326476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
@@ -7273,8 +7446,23 @@
         <f>AVERAGE(data!D2:D81)</f>
         <v>50248.035714285666</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>80</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>537.21785714285693</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>503.95714285714263</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>502.48035714285669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
@@ -7290,8 +7478,23 @@
         <f>AVERAGE(data!D2:D91)</f>
         <v>50062.063492063455</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>90</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>539.00952380952356</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>500.76349206349181</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>500.62063492063453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -7307,11 +7510,32 @@
         <f>AVERAGE(data!D2:D101)</f>
         <v>50203.285714285681</v>
       </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>540.35428571428531</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>499.6257142857142</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>502.03285714285681</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7319,8 +7543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="A9:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>